<commit_message>
Add prefilled league data
</commit_message>
<xml_diff>
--- a/public/data/clubs.xlsx
+++ b/public/data/clubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -41,6 +41,48 @@
   </si>
   <si>
     <t>activeContracts</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Premier Legue</t>
+  </si>
+  <si>
+    <t>/uploads/clubs/1766017335291-earth-23593_1280.png</t>
+  </si>
+  <si>
+    <t>man@gmail.com</t>
+  </si>
+  <si>
+    <t>+11 77 89834234</t>
+  </si>
+  <si>
+    <t>manchester.com</t>
+  </si>
+  <si>
+    <t>War Men</t>
+  </si>
+  <si>
+    <t>Freetown</t>
+  </si>
+  <si>
+    <t>Sierra Leone Premier</t>
+  </si>
+  <si>
+    <t>/uploads/clubs/1766018020521-Tom___Jerry.jpeg</t>
+  </si>
+  <si>
+    <t>warm@gmail.com</t>
+  </si>
+  <si>
+    <t>+323299888777</t>
+  </si>
+  <si>
+    <t>warm.com</t>
   </si>
 </sst>
 </file>
@@ -417,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -462,8 +504,72 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>